<commit_message>
schema: apply more default values
These are implied values as they are the defaults in the XSD
for optional attributes/elements. However I've noticed that
I keep running into issues where Mac Excel/Word fail to open
a file unless an optional default is provided.

I'll just add them all to hopefully increase compatibility and
save painful file format debugging sessions later.
</commit_message>
<xml_diff>
--- a/spreadsheet/testdata/simple-1.xlsx
+++ b/spreadsheet/testdata/simple-1.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
+<x:workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace" conformance="strict">
   <x:sheets>
-    <x:sheet name="Sheet 1" sheetId="1" r:id="rId3"/>
+    <x:sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId3"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -32,19 +32,19 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
+    <x:border outline="1">
+      <x:left style="none"/>
+      <x:right style="none"/>
+      <x:top style="none"/>
+      <x:bottom style="none"/>
+      <x:diagonal style="none"/>
     </x:border>
   </x:borders>
   <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" quotePrefix="0" pivotButton="0"/>
   </x:cellStyleXfs>
   <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -56,8 +56,8 @@
 <x:worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
   <x:dimension ref="A1"/>
   <x:sheetData>
-    <x:row r="1">
-      <x:c t="s">
+    <x:row r="1" s="0" customFormat="0" hidden="0" customHeight="0" outlineLevel="0" collapsed="0" thickTop="0" thickBot="0" ph="0">
+      <x:c s="0" t="s" cm="0" vm="0" ph="0">
         <x:v>0</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Revert "schema: apply more default values"
This caused problems with Libre.

This reverts commit 59b2711e1b87be534c9cd3d155710d13cfe7743b.
</commit_message>
<xml_diff>
--- a/spreadsheet/testdata/simple-1.xlsx
+++ b/spreadsheet/testdata/simple-1.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace" conformance="strict">
+<x:workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
   <x:sheets>
-    <x:sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId3"/>
+    <x:sheet name="Sheet 1" sheetId="1" r:id="rId3"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -32,19 +32,19 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border outline="1">
-      <x:left style="none"/>
-      <x:right style="none"/>
-      <x:top style="none"/>
-      <x:bottom style="none"/>
-      <x:diagonal style="none"/>
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
     </x:border>
   </x:borders>
   <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" quotePrefix="0" pivotButton="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </x:cellStyleXfs>
   <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -56,8 +56,8 @@
 <x:worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
   <x:dimension ref="A1"/>
   <x:sheetData>
-    <x:row r="1" s="0" customFormat="0" hidden="0" customHeight="0" outlineLevel="0" collapsed="0" thickTop="0" thickBot="0" ph="0">
-      <x:c s="0" t="s" cm="0" vm="0" ph="0">
+    <x:row r="1">
+      <x:c t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>

</xml_diff>